<commit_message>
Update convergence test analysis
</commit_message>
<xml_diff>
--- a/validation/vowels/resonances.xlsx
+++ b/validation/vowels/resonances.xlsx
@@ -15,99 +15,94 @@
     <sheet name="resonances" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">resonances!$B$12:$I$12</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">resonances!$B$13:$I$13</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">resonances!$B$79:$I$79</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">resonances!$B$80:$I$80</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">resonances!$B$81:$I$81</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">resonances!$B$25:$I$25</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">resonances!$B$26:$I$26</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">resonances!$B$27:$I$27</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">resonances!$B$28:$I$28</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">resonances!$B$151:$L$151</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">resonances!$B$152:$L$152</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">resonances!$B$153:$L$153</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">resonances!$B$14:$I$14</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">resonances!$B$154:$L$154</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">resonances!$B$61:$I$61</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">resonances!$B$62:$I$62</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">resonances!$B$63:$I$63</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">resonances!$B$64:$I$64</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">resonances!$B$43:$I$43</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">resonances!$B$44:$I$44</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">resonances!$B$45:$I$45</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">resonances!$B$46:$I$46</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">resonances!$B$10:$I$10</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">resonances!$B$15:$I$15</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">resonances!$B$7:$I$7</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">resonances!$B$8:$I$8</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">resonances!$B$9:$I$9</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">resonances!$B$96:$I$96</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">resonances!$B$97:$I$97</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">resonances!$B$98:$I$98</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">resonances!$B$99:$I$99</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">resonances!$B$66:$I$66</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">resonances!$B$67:$I$67</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">resonances!$B$68:$I$68</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">resonances!$B$16:$I$16</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">resonances!$B$69:$I$69</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">resonances!$B$70:$I$70</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">resonances!$B$83:$I$83</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">resonances!$B$84:$I$84</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">resonances!$B$85:$I$85</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">resonances!$B$86:$I$86</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">resonances!$B$87:$I$87</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">resonances!$B$48:$I$48</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">resonances!$B$49:$I$49</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">resonances!$B$50:$I$50</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">resonances!$B$114:$L$114</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">resonances!$B$51:$I$51</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">resonances!$B$52:$I$52</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">resonances!$B$30:$I$30</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">resonances!$B$31:$I$31</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">resonances!$B$32:$I$32</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">resonances!$B$33:$I$33</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">resonances!$B$34:$I$34</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">resonances!$B$101:$I$101</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">resonances!$B$102:$I$102</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">resonances!$B$103:$I$103</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">resonances!$B$115:$L$115</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">resonances!$B$104:$I$104</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">resonances!$B$105:$I$105</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">resonances!$B$132:$L$132</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">resonances!$B$133:$L$133</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">resonances!$B$134:$L$134</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">resonances!$B$135:$L$135</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">resonances!$B$156:$L$156</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">resonances!$B$157:$L$157</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">resonances!$B$158:$L$158</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">resonances!$B$159:$L$159</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">resonances!$B$116:$L$116</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">resonances!$B$160:$L$160</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">resonances!$B$156:$L$156</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">resonances!$B$157:$L$157</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">resonances!$B$158:$L$158</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">resonances!$B$159:$L$159</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">resonances!$B$160:$L$160</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">resonances!$B$137:$L$137</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">resonances!$B$138:$L$138</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">resonances!$B$139:$L$139</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">resonances!$B$140:$L$140</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">resonances!$B$117:$L$117</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">resonances!$B$141:$L$141</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">resonances!$B$119:$L$119</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">resonances!$B$120:$L$120</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">resonances!$B$121:$L$121</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">resonances!$B$122:$L$122</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">resonances!$B$123:$L$123</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">resonances!$B$78:$I$78</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">resonances!$B$43:$I$43</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">resonances!$B$44:$I$44</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">resonances!$B$27:$I$27</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">resonances!$B$28:$I$28</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">resonances!$B$78:$I$78</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">resonances!$B$79:$I$79</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">resonances!$B$80:$I$80</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">resonances!$B$81:$I$81</definedName>
+    <definedName name="_xlchart.v1.16" hidden="1">resonances!$B$96:$I$96</definedName>
+    <definedName name="_xlchart.v1.17" hidden="1">resonances!$B$97:$I$97</definedName>
+    <definedName name="_xlchart.v1.18" hidden="1">resonances!$B$98:$I$98</definedName>
+    <definedName name="_xlchart.v1.19" hidden="1">resonances!$B$99:$I$99</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">resonances!$B$45:$I$45</definedName>
+    <definedName name="_xlchart.v1.20" hidden="1">resonances!$B$151:$L$151</definedName>
+    <definedName name="_xlchart.v1.21" hidden="1">resonances!$B$152:$L$152</definedName>
+    <definedName name="_xlchart.v1.22" hidden="1">resonances!$B$153:$L$153</definedName>
+    <definedName name="_xlchart.v1.23" hidden="1">resonances!$B$154:$L$154</definedName>
+    <definedName name="_xlchart.v1.24" hidden="1">resonances!$B$132:$L$132</definedName>
+    <definedName name="_xlchart.v1.25" hidden="1">resonances!$B$133:$L$133</definedName>
+    <definedName name="_xlchart.v1.26" hidden="1">resonances!$B$134:$L$134</definedName>
+    <definedName name="_xlchart.v1.27" hidden="1">resonances!$B$135:$L$135</definedName>
+    <definedName name="_xlchart.v1.28" hidden="1">resonances!$B$12:$I$12</definedName>
+    <definedName name="_xlchart.v1.29" hidden="1">resonances!$B$13:$I$13</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">resonances!$B$46:$I$46</definedName>
+    <definedName name="_xlchart.v1.30" hidden="1">resonances!$B$14:$I$14</definedName>
+    <definedName name="_xlchart.v1.31" hidden="1">resonances!$B$15:$I$15</definedName>
+    <definedName name="_xlchart.v1.32" hidden="1">resonances!$B$16:$I$16</definedName>
+    <definedName name="_xlchart.v1.33" hidden="1">resonances!$B$114:$L$114</definedName>
+    <definedName name="_xlchart.v1.34" hidden="1">resonances!$B$115:$L$115</definedName>
+    <definedName name="_xlchart.v1.35" hidden="1">resonances!$B$116:$L$116</definedName>
+    <definedName name="_xlchart.v1.36" hidden="1">resonances!$B$117:$L$117</definedName>
+    <definedName name="_xlchart.v1.37" hidden="1">resonances!$B$30:$I$30</definedName>
+    <definedName name="_xlchart.v1.38" hidden="1">resonances!$B$31:$I$31</definedName>
+    <definedName name="_xlchart.v1.39" hidden="1">resonances!$B$32:$I$32</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">resonances!$B$61:$I$61</definedName>
+    <definedName name="_xlchart.v1.40" hidden="1">resonances!$B$33:$I$33</definedName>
+    <definedName name="_xlchart.v1.41" hidden="1">resonances!$B$34:$I$34</definedName>
+    <definedName name="_xlchart.v1.42" hidden="1">resonances!$B$48:$I$48</definedName>
+    <definedName name="_xlchart.v1.43" hidden="1">resonances!$B$49:$I$49</definedName>
+    <definedName name="_xlchart.v1.44" hidden="1">resonances!$B$50:$I$50</definedName>
+    <definedName name="_xlchart.v1.45" hidden="1">resonances!$B$51:$I$51</definedName>
+    <definedName name="_xlchart.v1.46" hidden="1">resonances!$B$52:$I$52</definedName>
+    <definedName name="_xlchart.v1.47" hidden="1">resonances!$B$101:$I$101</definedName>
+    <definedName name="_xlchart.v1.48" hidden="1">resonances!$B$102:$I$102</definedName>
+    <definedName name="_xlchart.v1.49" hidden="1">resonances!$B$103:$I$103</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">resonances!$B$62:$I$62</definedName>
+    <definedName name="_xlchart.v1.50" hidden="1">resonances!$B$104:$I$104</definedName>
+    <definedName name="_xlchart.v1.51" hidden="1">resonances!$B$105:$I$105</definedName>
+    <definedName name="_xlchart.v1.52" hidden="1">resonances!$B$119:$L$119</definedName>
+    <definedName name="_xlchart.v1.53" hidden="1">resonances!$B$120:$L$120</definedName>
+    <definedName name="_xlchart.v1.54" hidden="1">resonances!$B$121:$L$121</definedName>
+    <definedName name="_xlchart.v1.55" hidden="1">resonances!$B$122:$L$122</definedName>
+    <definedName name="_xlchart.v1.56" hidden="1">resonances!$B$123:$L$123</definedName>
+    <definedName name="_xlchart.v1.57" hidden="1">resonances!$B$83:$I$83</definedName>
+    <definedName name="_xlchart.v1.58" hidden="1">resonances!$B$84:$I$84</definedName>
+    <definedName name="_xlchart.v1.59" hidden="1">resonances!$B$85:$I$85</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">resonances!$B$63:$I$63</definedName>
+    <definedName name="_xlchart.v1.60" hidden="1">resonances!$B$86:$I$86</definedName>
+    <definedName name="_xlchart.v1.61" hidden="1">resonances!$B$87:$I$87</definedName>
+    <definedName name="_xlchart.v1.62" hidden="1">resonances!$B$137:$L$137</definedName>
+    <definedName name="_xlchart.v1.63" hidden="1">resonances!$B$138:$L$138</definedName>
+    <definedName name="_xlchart.v1.64" hidden="1">resonances!$B$139:$L$139</definedName>
+    <definedName name="_xlchart.v1.65" hidden="1">resonances!$B$140:$L$140</definedName>
+    <definedName name="_xlchart.v1.66" hidden="1">resonances!$B$141:$L$141</definedName>
+    <definedName name="_xlchart.v1.67" hidden="1">resonances!$B$66:$I$66</definedName>
+    <definedName name="_xlchart.v1.68" hidden="1">resonances!$B$67:$I$67</definedName>
+    <definedName name="_xlchart.v1.69" hidden="1">resonances!$B$68:$I$68</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">resonances!$B$64:$I$64</definedName>
+    <definedName name="_xlchart.v1.70" hidden="1">resonances!$B$69:$I$69</definedName>
+    <definedName name="_xlchart.v1.71" hidden="1">resonances!$B$70:$I$70</definedName>
+    <definedName name="_xlchart.v1.72" hidden="1">resonances!$B$156:$L$156</definedName>
+    <definedName name="_xlchart.v1.73" hidden="1">resonances!$B$157:$L$157</definedName>
+    <definedName name="_xlchart.v1.74" hidden="1">resonances!$B$158:$L$158</definedName>
+    <definedName name="_xlchart.v1.75" hidden="1">resonances!$B$159:$L$159</definedName>
+    <definedName name="_xlchart.v1.76" hidden="1">resonances!$B$160:$L$160</definedName>
+    <definedName name="_xlchart.v1.77" hidden="1">resonances!$B$10:$I$10</definedName>
+    <definedName name="_xlchart.v1.78" hidden="1">resonances!$B$7:$I$7</definedName>
+    <definedName name="_xlchart.v1.79" hidden="1">resonances!$B$8:$I$8</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">resonances!$B$25:$I$25</definedName>
+    <definedName name="_xlchart.v1.80" hidden="1">resonances!$B$9:$I$9</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">resonances!$B$26:$I$26</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
   <si>
     <t>Vowel a</t>
   </si>
@@ -132,13 +127,25 @@
   <si>
     <t>corr shift</t>
   </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -647,7 +654,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -713,51 +720,68 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.30</cx:f>
+        <cx:f dir="row">_xlchart.v1.8</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.31</cx:f>
+        <cx:f dir="row">_xlchart.v1.9</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.32</cx:f>
+        <cx:f dir="row">_xlchart.v1.10</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.29</cx:f>
+        <cx:f dir="row">_xlchart.v1.11</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Diagrammtitel</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{08BC4EA7-6596-4BC2-BC56-562457E6B5EA}">
+        <cx:series layoutId="boxWhisker" uniqueId="{C785EE48-C10C-4FF0-BE09-0ADE4AA48704}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{7E7A1411-CAB1-46A6-97AA-E62BAB4E2446}">
+        <cx:series layoutId="boxWhisker" uniqueId="{9E6B7963-DE0B-46EE-8D8F-C013B8B4FAFF}">
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{465EE7B8-DDB4-4AF0-8029-783AF821EE32}">
+        <cx:series layoutId="boxWhisker" uniqueId="{8D8E8ACD-0CA3-407F-AE77-C6FDE275AA53}">
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{4D103E40-17FE-4281-B041-85EE3C6FD4BE}">
+        <cx:series layoutId="boxWhisker" uniqueId="{B5607A0C-C45E-42D0-B1C3-E807735B5CD4}">
           <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -784,115 +808,49 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.0</cx:f>
+        <cx:f dir="row">_xlchart.v1.37</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.1</cx:f>
+        <cx:f dir="row">_xlchart.v1.38</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.2</cx:f>
+        <cx:f dir="row">_xlchart.v1.39</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.3</cx:f>
+        <cx:f dir="row">_xlchart.v1.40</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.4</cx:f>
+        <cx:f dir="row">_xlchart.v1.41</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
-    <cx:plotArea>
-      <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{9274DD3C-7FA8-4213-B3B7-D1EC758427F3}">
-          <cx:dataId val="0"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{C672D788-294F-495C-AA54-713563ECEE8C}">
-          <cx:dataId val="1"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{2CF54D97-3583-4F99-8606-F59FB4DA3E1A}">
-          <cx:dataId val="2"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{9F699736-B320-4A46-9D2B-BD83BDA4773B}">
-          <cx:dataId val="3"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{06728016-5ACD-42E9-88F0-4B7BE4C66912}">
-          <cx:dataId val="4"/>
-          <cx:layoutPr>
-            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
-            <cx:statistics quartileMethod="exclusive"/>
-          </cx:layoutPr>
-        </cx:series>
-      </cx:plotAreaRegion>
-      <cx:axis id="0">
-        <cx:catScaling gapWidth="1"/>
-        <cx:tickLabels/>
-      </cx:axis>
-      <cx:axis id="1">
-        <cx:valScaling/>
-        <cx:majorGridlines/>
-        <cx:tickLabels/>
-      </cx:axis>
-    </cx:plotArea>
-  </cx:chart>
-</cx:chartSpace>
-</file>
-
-<file path=xl/charts/chartEx11.xml><?xml version="1.0" encoding="utf-8"?>
-<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
-  <cx:chartData>
-    <cx:data id="0">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.52</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="1">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.53</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="2">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.54</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="3">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.55</cx:f>
-      </cx:numDim>
-    </cx:data>
-    <cx:data id="4">
-      <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.56</cx:f>
-      </cx:numDim>
-    </cx:data>
-  </cx:chartData>
-  <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Diagrammtitel</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{BAAB8583-06C1-475D-90CD-5F3D5C9D4451}">
@@ -945,37 +903,53 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx11.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.47</cx:f>
+        <cx:f dir="row">_xlchart.v1.42</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.48</cx:f>
+        <cx:f dir="row">_xlchart.v1.43</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.49</cx:f>
+        <cx:f dir="row">_xlchart.v1.44</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.50</cx:f>
+        <cx:f dir="row">_xlchart.v1.45</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.51</cx:f>
+        <cx:f dir="row">_xlchart.v1.46</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Diagrammtitel</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{B8824406-7D8A-41B2-AF42-1E8CB344F729}">
@@ -1028,37 +1002,73 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx12.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.37</cx:f>
+        <cx:f dir="row">_xlchart.v1.67</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.38</cx:f>
+        <cx:f dir="row">_xlchart.v1.68</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.39</cx:f>
+        <cx:f dir="row">_xlchart.v1.69</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.40</cx:f>
+        <cx:f dir="row">_xlchart.v1.70</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.41</cx:f>
+        <cx:f dir="row">_xlchart.v1.71</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>i</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FEM</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{29002219-B05B-461A-8D47-1DD5E83DA9BB}">
@@ -1111,32 +1121,32 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx13.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.42</cx:f>
+        <cx:f dir="row">_xlchart.v1.57</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.43</cx:f>
+        <cx:f dir="row">_xlchart.v1.58</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.44</cx:f>
+        <cx:f dir="row">_xlchart.v1.59</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.45</cx:f>
+        <cx:f dir="row">_xlchart.v1.60</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.46</cx:f>
+        <cx:f dir="row">_xlchart.v1.61</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1194,32 +1204,32 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx14.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.57</cx:f>
+        <cx:f dir="row">_xlchart.v1.47</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.58</cx:f>
+        <cx:f dir="row">_xlchart.v1.48</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.59</cx:f>
+        <cx:f dir="row">_xlchart.v1.49</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.60</cx:f>
+        <cx:f dir="row">_xlchart.v1.50</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.61</cx:f>
+        <cx:f dir="row">_xlchart.v1.51</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1277,32 +1287,32 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx15.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.76</cx:f>
+        <cx:f dir="row">_xlchart.v1.62</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.77</cx:f>
+        <cx:f dir="row">_xlchart.v1.63</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.78</cx:f>
+        <cx:f dir="row">_xlchart.v1.64</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.79</cx:f>
+        <cx:f dir="row">_xlchart.v1.65</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.80</cx:f>
+        <cx:f dir="row">_xlchart.v1.66</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1360,37 +1370,73 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx16.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.81</cx:f>
+        <cx:f dir="row">_xlchart.v1.52</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.82</cx:f>
+        <cx:f dir="row">_xlchart.v1.53</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.83</cx:f>
+        <cx:f dir="row">_xlchart.v1.54</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.84</cx:f>
+        <cx:f dir="row">_xlchart.v1.55</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.85</cx:f>
+        <cx:f dir="row">_xlchart.v1.56</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>u</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FEM</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{331FECF5-4807-489D-994A-F79C61D71E66}">
@@ -1443,32 +1489,32 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx17.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.66</cx:f>
+        <cx:f dir="row">_xlchart.v1.72</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.67</cx:f>
+        <cx:f dir="row">_xlchart.v1.73</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.68</cx:f>
+        <cx:f dir="row">_xlchart.v1.74</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.69</cx:f>
+        <cx:f dir="row">_xlchart.v1.75</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="4">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.70</cx:f>
+        <cx:f dir="row">_xlchart.v1.76</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1526,56 +1572,100 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx18.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.13</cx:f>
+        <cx:f dir="row">_xlchart.v1.78</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.14</cx:f>
+        <cx:f dir="row">_xlchart.v1.79</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.15</cx:f>
+        <cx:f dir="row">_xlchart.v1.80</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.16</cx:f>
+        <cx:f dir="row">_xlchart.v1.77</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>a</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>6</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>0</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> kHz</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
-        <cx:series layoutId="boxWhisker" uniqueId="{C785EE48-C10C-4FF0-BE09-0ADE4AA48704}">
+        <cx:series layoutId="boxWhisker" uniqueId="{6F086EAB-CFA2-4274-854F-809AC7AA7D48}">
           <cx:dataId val="0"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{9E6B7963-DE0B-46EE-8D8F-C013B8B4FAFF}">
+        <cx:series layoutId="boxWhisker" uniqueId="{195CFD01-F527-4F21-873F-4DECF0499ED1}">
           <cx:dataId val="1"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{8D8E8ACD-0CA3-407F-AE77-C6FDE275AA53}">
+        <cx:series layoutId="boxWhisker" uniqueId="{6C133B3F-F9E9-4C7B-B269-4CFA8B6963F4}">
           <cx:dataId val="2"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
           </cx:layoutPr>
         </cx:series>
-        <cx:series layoutId="boxWhisker" uniqueId="{B5607A0C-C45E-42D0-B1C3-E807735B5CD4}">
+        <cx:series layoutId="boxWhisker" uniqueId="{6067F4B0-93B5-45D6-84FD-59A9F3402AAA}">
           <cx:dataId val="3"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
@@ -1597,32 +1687,49 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx2.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.25</cx:f>
+        <cx:f dir="row">_xlchart.v1.0</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.26</cx:f>
+        <cx:f dir="row">_xlchart.v1.1</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.27</cx:f>
+        <cx:f dir="row">_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.28</cx:f>
+        <cx:f dir="row">_xlchart.v1.3</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Diagrammtitel</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{424C8B0D-F5DF-4D00-B6D1-9C758D21C1F8}">
@@ -1668,32 +1775,77 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.21</cx:f>
+        <cx:f dir="row">_xlchart.v1.4</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.22</cx:f>
+        <cx:f dir="row">_xlchart.v1.5</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.23</cx:f>
+        <cx:f dir="row">_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.24</cx:f>
+        <cx:f dir="row">_xlchart.v1.7</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>i</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>6</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>0</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> kHz</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{28EB4745-0E55-4018-B60B-26F10869D356}">
@@ -1739,27 +1891,27 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx4.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.9</cx:f>
+        <cx:f dir="row">_xlchart.v1.12</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.10</cx:f>
+        <cx:f dir="row">_xlchart.v1.13</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.11</cx:f>
+        <cx:f dir="row">_xlchart.v1.14</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.12</cx:f>
+        <cx:f dir="row">_xlchart.v1.15</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1810,27 +1962,27 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx5.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.33</cx:f>
+        <cx:f dir="row">_xlchart.v1.16</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.34</cx:f>
+        <cx:f dir="row">_xlchart.v1.17</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.35</cx:f>
+        <cx:f dir="row">_xlchart.v1.18</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.36</cx:f>
+        <cx:f dir="row">_xlchart.v1.19</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -1881,32 +2033,76 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx6.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.5</cx:f>
+        <cx:f dir="row">_xlchart.v1.33</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.6</cx:f>
+        <cx:f dir="row">_xlchart.v1.34</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.7</cx:f>
+        <cx:f dir="row">_xlchart.v1.35</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.8</cx:f>
+        <cx:f dir="row">_xlchart.v1.36</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
   <cx:chart>
-    <cx:title pos="t" align="ctr" overlay="0"/>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>u</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>6</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>0</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> kHz</a:t>
+            </a:r>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
     <cx:plotArea>
       <cx:plotAreaRegion>
         <cx:series layoutId="boxWhisker" uniqueId="{8CB44AD6-D05E-4056-81E4-2B26437DF630}">
@@ -1952,27 +2148,27 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx7.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.62</cx:f>
+        <cx:f dir="row">_xlchart.v1.24</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.63</cx:f>
+        <cx:f dir="row">_xlchart.v1.25</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.64</cx:f>
+        <cx:f dir="row">_xlchart.v1.26</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.65</cx:f>
+        <cx:f dir="row">_xlchart.v1.27</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2023,27 +2219,27 @@
 </cx:chartSpace>
 </file>
 
-<file path=xl/charts/chartEx9.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chartEx8.xml><?xml version="1.0" encoding="utf-8"?>
 <cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
   <cx:chartData>
     <cx:data id="0">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.17</cx:f>
+        <cx:f dir="row">_xlchart.v1.20</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="1">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.18</cx:f>
+        <cx:f dir="row">_xlchart.v1.21</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="2">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.19</cx:f>
+        <cx:f dir="row">_xlchart.v1.22</cx:f>
       </cx:numDim>
     </cx:data>
     <cx:data id="3">
       <cx:numDim type="val">
-        <cx:f dir="row">_xlchart.v1.20</cx:f>
+        <cx:f dir="row">_xlchart.v1.23</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -2074,6 +2270,126 @@
         </cx:series>
         <cx:series layoutId="boxWhisker" uniqueId="{00A0BA87-4F2A-4EF3-AA4D-647A753B89D1}">
           <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="1"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx9.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.28</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="1">
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.29</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="2">
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.30</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="3">
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.31</cx:f>
+      </cx:numDim>
+    </cx:data>
+    <cx:data id="4">
+      <cx:numDim type="val">
+        <cx:f dir="row">_xlchart.v1.32</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr algn="ctr">
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>a</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t>/</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t> ref</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-DE"/>
+              <a:t> </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>FEM</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-DE"/>
+          </a:p>
+        </cx:rich>
+      </cx:tx>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="boxWhisker" uniqueId="{9274DD3C-7FA8-4213-B3B7-D1EC758427F3}">
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{C672D788-294F-495C-AA54-713563ECEE8C}">
+          <cx:dataId val="1"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{2CF54D97-3583-4F99-8606-F59FB4DA3E1A}">
+          <cx:dataId val="2"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{9F699736-B320-4A46-9D2B-BD83BDA4773B}">
+          <cx:dataId val="3"/>
+          <cx:layoutPr>
+            <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
+            <cx:statistics quartileMethod="exclusive"/>
+          </cx:layoutPr>
+        </cx:series>
+        <cx:series layoutId="boxWhisker" uniqueId="{06728016-5ACD-42E9-88F0-4B7BE4C66912}">
+          <cx:dataId val="4"/>
           <cx:layoutPr>
             <cx:visibility meanLine="0" meanMarker="1" nonoutliers="0" outliers="1"/>
             <cx:statistics quartileMethod="exclusive"/>
@@ -11567,74 +11883,6 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>238126</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>104774</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
-        <xdr:graphicFrame macro="">
-          <xdr:nvGraphicFramePr>
-            <xdr:cNvPr id="2" name="Diagramm 1"/>
-            <xdr:cNvGraphicFramePr/>
-          </xdr:nvGraphicFramePr>
-          <xdr:xfrm>
-            <a:off x="0" y="0"/>
-            <a:ext cx="0" cy="0"/>
-          </xdr:xfrm>
-          <a:graphic>
-            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-            </a:graphicData>
-          </a:graphic>
-        </xdr:graphicFrame>
-      </mc:Choice>
-      <mc:Fallback>
-        <xdr:sp macro="" textlink="">
-          <xdr:nvSpPr>
-            <xdr:cNvPr id="0" name=""/>
-            <xdr:cNvSpPr>
-              <a:spLocks noTextEdit="1"/>
-            </xdr:cNvSpPr>
-          </xdr:nvSpPr>
-          <xdr:spPr>
-            <a:prstGeom prst="rect">
-              <a:avLst/>
-            </a:prstGeom>
-            <a:solidFill>
-              <a:prstClr val="white"/>
-            </a:solidFill>
-            <a:ln w="1">
-              <a:solidFill>
-                <a:prstClr val="green"/>
-              </a:solidFill>
-            </a:ln>
-          </xdr:spPr>
-          <xdr:txBody>
-            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:r>
-                <a:rPr lang="en-GB" sz="1100"/>
-                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
-Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
-              </a:r>
-            </a:p>
-          </xdr:txBody>
-        </xdr:sp>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
       <xdr:colOff>257175</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>95250</xdr:rowOff>
@@ -11658,7 +11906,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -11726,7 +11974,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -11776,10 +12024,10 @@
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>171450</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -11794,7 +12042,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -11862,7 +12110,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -11930,7 +12178,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -11977,13 +12225,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>133350</xdr:colOff>
       <xdr:row>106</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:rowOff>180976</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>38100</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>742950</xdr:colOff>
+      <xdr:row>117</xdr:row>
+      <xdr:rowOff>171450</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -11998,7 +12246,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId6"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12066,7 +12314,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId7"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12134,7 +12382,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId8"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12178,16 +12426,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>95251</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>542924</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>114301</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -12202,7 +12450,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId9"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12270,7 +12518,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId10"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12338,7 +12586,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId11"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12388,10 +12636,10 @@
       <xdr:rowOff>66674</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>69</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -12406,7 +12654,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId12"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12474,7 +12722,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId13"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12542,7 +12790,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId14"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12610,7 +12858,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId15"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12660,10 +12908,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>123825</xdr:colOff>
-      <xdr:row>124</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>118</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -12678,7 +12926,7 @@
           </xdr:xfrm>
           <a:graphic>
             <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
-              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId16"/>
             </a:graphicData>
           </a:graphic>
         </xdr:graphicFrame>
@@ -12738,6 +12986,74 @@
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="19" name="Diagramm 18"/>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId17"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="en-GB" sz="1100"/>
+                <a:t>Dieses Diagramm ist in Ihrer Version von Excel nicht verfügbar.
+Wenn Sie diese Form bearbeiten oder diese Arbeitsmappe in einem anderen Dateiformat speichern, wird das Diagramm dauerhaft beschädigt.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>561974</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>542925</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="20" name="Diagramm 19"/>
             <xdr:cNvGraphicFramePr/>
           </xdr:nvGraphicFramePr>
           <xdr:xfrm>
@@ -13054,10 +13370,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N160"/>
+  <dimension ref="A1:N161"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A156" sqref="A156:A160"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13232,6 +13548,9 @@
       </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>8</v>
+      </c>
       <c r="B7" s="3">
         <f>100*ABS(B6-B2)/B6</f>
         <v>1.7001545595054095</v>
@@ -13274,6 +13593,9 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
       <c r="B8" s="3">
         <f>100*ABS(B6-B3)/B6</f>
         <v>0.92735703245749612</v>
@@ -13316,6 +13638,9 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
       <c r="B9" s="3">
         <f>100*ABS(B6-B4)/B6</f>
         <v>0.46367851622874806</v>
@@ -13358,6 +13683,9 @@
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
       <c r="B10" s="3">
         <f>100*ABS(B6-B5)/B6</f>
         <v>0.15455950540958269</v>
@@ -17775,27 +18103,27 @@
         <v>20</v>
       </c>
       <c r="B137" s="2">
-        <f>100*ABS(B$136-B127)/B$136</f>
+        <f t="shared" ref="B137:G141" si="140">100*ABS(B$136-B127)/B$136</f>
         <v>8.9552238805970141</v>
       </c>
       <c r="C137" s="2">
-        <f>100*ABS(C$136-C127)/C$136</f>
+        <f t="shared" si="140"/>
         <v>20</v>
       </c>
       <c r="D137" s="2">
-        <f>100*ABS(D$136-D127)/D$136</f>
+        <f t="shared" si="140"/>
         <v>10.1010101010101</v>
       </c>
       <c r="E137" s="2">
-        <f>100*ABS(E$136-E127)/E$136</f>
+        <f t="shared" si="140"/>
         <v>5.645161290322581</v>
       </c>
       <c r="F137" s="2">
-        <f>100*ABS(F$136-F127)/F$136</f>
+        <f t="shared" si="140"/>
         <v>16.346153846153847</v>
       </c>
       <c r="G137" s="2">
-        <f>100*ABS(G$136-G127)/G$136</f>
+        <f t="shared" si="140"/>
         <v>12.222222222222221</v>
       </c>
       <c r="H137" s="2"/>
@@ -17810,11 +18138,11 @@
         <v>10.76923076923077</v>
       </c>
       <c r="M137" s="3">
-        <f t="shared" ref="M137" si="140">MAX(E137:L137)</f>
+        <f t="shared" ref="M137" si="141">MAX(E137:L137)</f>
         <v>16.346153846153847</v>
       </c>
       <c r="N137" s="3">
-        <f t="shared" ref="N137" si="141">AVERAGE(E137:L137)</f>
+        <f t="shared" ref="N137" si="142">AVERAGE(E137:L137)</f>
         <v>9.3763004610289222</v>
       </c>
     </row>
@@ -17823,27 +18151,27 @@
         <v>30</v>
       </c>
       <c r="B138" s="2">
-        <f>100*ABS(B$136-B128)/B$136</f>
+        <f t="shared" si="140"/>
         <v>7.4626865671641793</v>
       </c>
       <c r="C138" s="2">
-        <f>100*ABS(C$136-C128)/C$136</f>
+        <f t="shared" si="140"/>
         <v>21.25</v>
       </c>
       <c r="D138" s="2">
-        <f>100*ABS(D$136-D128)/D$136</f>
+        <f t="shared" si="140"/>
         <v>10.1010101010101</v>
       </c>
       <c r="E138" s="2">
-        <f>100*ABS(E$136-E128)/E$136</f>
+        <f t="shared" si="140"/>
         <v>8.064516129032258</v>
       </c>
       <c r="F138" s="2">
-        <f>100*ABS(F$136-F128)/F$136</f>
+        <f t="shared" si="140"/>
         <v>15.384615384615385</v>
       </c>
       <c r="G138" s="2">
-        <f>100*ABS(G$136-G128)/G$136</f>
+        <f t="shared" si="140"/>
         <v>11.111111111111111</v>
       </c>
       <c r="H138" s="2"/>
@@ -17858,11 +18186,11 @@
       <c r="K138" s="2"/>
       <c r="L138" s="2"/>
       <c r="M138" s="3">
-        <f t="shared" ref="M138:M141" si="142">MAX(E138:L138)</f>
+        <f t="shared" ref="M138:M141" si="143">MAX(E138:L138)</f>
         <v>20.666666666666668</v>
       </c>
       <c r="N138" s="3">
-        <f t="shared" ref="N138:N141" si="143">AVERAGE(E138:L138)</f>
+        <f t="shared" ref="N138:N141" si="144">AVERAGE(E138:L138)</f>
         <v>13.197280592462301</v>
       </c>
     </row>
@@ -17871,27 +18199,27 @@
         <v>40</v>
       </c>
       <c r="B139" s="2">
-        <f>100*ABS(B$136-B129)/B$136</f>
+        <f t="shared" si="140"/>
         <v>8.9552238805970141</v>
       </c>
       <c r="C139" s="2">
-        <f>100*ABS(C$136-C129)/C$136</f>
+        <f t="shared" si="140"/>
         <v>21.25</v>
       </c>
       <c r="D139" s="2">
-        <f>100*ABS(D$136-D129)/D$136</f>
+        <f t="shared" si="140"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="E139" s="2">
-        <f>100*ABS(E$136-E129)/E$136</f>
+        <f t="shared" si="140"/>
         <v>3.225806451612903</v>
       </c>
       <c r="F139" s="2">
-        <f>100*ABS(F$136-F129)/F$136</f>
+        <f t="shared" si="140"/>
         <v>18.26923076923077</v>
       </c>
       <c r="G139" s="2">
-        <f>100*ABS(G$136-G129)/G$136</f>
+        <f t="shared" si="140"/>
         <v>12.222222222222221</v>
       </c>
       <c r="H139" s="2"/>
@@ -17909,11 +18237,11 @@
         <v>8.4615384615384617</v>
       </c>
       <c r="M139" s="3">
-        <f t="shared" si="142"/>
+        <f t="shared" si="143"/>
         <v>24.666666666666668</v>
       </c>
       <c r="N139" s="3">
-        <f t="shared" si="143"/>
+        <f t="shared" si="144"/>
         <v>13.778041563566269</v>
       </c>
     </row>
@@ -17922,27 +18250,27 @@
         <v>50</v>
       </c>
       <c r="B140" s="2">
-        <f>100*ABS(B$136-B130)/B$136</f>
+        <f t="shared" si="140"/>
         <v>7.4626865671641793</v>
       </c>
       <c r="C140" s="2">
-        <f>100*ABS(C$136-C130)/C$136</f>
+        <f t="shared" si="140"/>
         <v>21.25</v>
       </c>
       <c r="D140" s="2">
-        <f>100*ABS(D$136-D130)/D$136</f>
+        <f t="shared" si="140"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="E140" s="2">
-        <f>100*ABS(E$136-E130)/E$136</f>
+        <f t="shared" si="140"/>
         <v>2.4193548387096775</v>
       </c>
       <c r="F140" s="2">
-        <f>100*ABS(F$136-F130)/F$136</f>
+        <f t="shared" si="140"/>
         <v>18.26923076923077</v>
       </c>
       <c r="G140" s="2">
-        <f>100*ABS(G$136-G130)/G$136</f>
+        <f t="shared" si="140"/>
         <v>12.222222222222221</v>
       </c>
       <c r="H140" s="2"/>
@@ -17960,11 +18288,11 @@
         <v>7.6923076923076925</v>
       </c>
       <c r="M140" s="3">
-        <f t="shared" si="142"/>
+        <f t="shared" si="143"/>
         <v>26</v>
       </c>
       <c r="N140" s="3">
-        <f t="shared" si="143"/>
+        <f t="shared" si="144"/>
         <v>14.265076215770376</v>
       </c>
     </row>
@@ -17973,27 +18301,27 @@
         <v>60</v>
       </c>
       <c r="B141" s="2">
-        <f>100*ABS(B$136-B131)/B$136</f>
+        <f t="shared" si="140"/>
         <v>8.9552238805970141</v>
       </c>
       <c r="C141" s="2">
-        <f>100*ABS(C$136-C131)/C$136</f>
+        <f t="shared" si="140"/>
         <v>21.25</v>
       </c>
       <c r="D141" s="2">
-        <f>100*ABS(D$136-D131)/D$136</f>
+        <f t="shared" si="140"/>
         <v>6.0606060606060606</v>
       </c>
       <c r="E141" s="2">
-        <f>100*ABS(E$136-E131)/E$136</f>
+        <f t="shared" si="140"/>
         <v>3.225806451612903</v>
       </c>
       <c r="F141" s="2">
-        <f>100*ABS(F$136-F131)/F$136</f>
+        <f t="shared" si="140"/>
         <v>18.26923076923077</v>
       </c>
       <c r="G141" s="2">
-        <f>100*ABS(G$136-G131)/G$136</f>
+        <f t="shared" si="140"/>
         <v>12.222222222222221</v>
       </c>
       <c r="H141" s="2"/>
@@ -18011,11 +18339,11 @@
         <v>8.4615384615384617</v>
       </c>
       <c r="M141" s="3">
-        <f t="shared" si="142"/>
+        <f t="shared" si="143"/>
         <v>24</v>
       </c>
       <c r="N141" s="3">
-        <f t="shared" si="143"/>
+        <f t="shared" si="144"/>
         <v>14.19435661279271</v>
       </c>
     </row>
@@ -18245,36 +18573,36 @@
         <v>0.53521064916580363</v>
       </c>
       <c r="C151" s="3">
-        <f t="shared" ref="C151" si="144">100*ABS(C150-C146)/C150</f>
+        <f t="shared" ref="C151" si="145">100*ABS(C150-C146)/C150</f>
         <v>0.20596795528546066</v>
       </c>
       <c r="D151" s="3">
-        <f t="shared" ref="D151" si="145">100*ABS(D150-D146)/D150</f>
+        <f t="shared" ref="D151" si="146">100*ABS(D150-D146)/D150</f>
         <v>3.487434383136049</v>
       </c>
       <c r="E151" s="3">
-        <f t="shared" ref="E151" si="146">100*ABS(E150-E146)/E150</f>
+        <f t="shared" ref="E151" si="147">100*ABS(E150-E146)/E150</f>
         <v>12.226026249115968</v>
       </c>
       <c r="F151" s="3">
-        <f t="shared" ref="F151" si="147">100*ABS(F150-F146)/F150</f>
+        <f t="shared" ref="F151" si="148">100*ABS(F150-F146)/F150</f>
         <v>12.081356600779126</v>
       </c>
       <c r="G151" s="3">
-        <f t="shared" ref="G151" si="148">100*ABS(G150-G146)/G150</f>
+        <f t="shared" ref="G151" si="149">100*ABS(G150-G146)/G150</f>
         <v>2.2554794689781246</v>
       </c>
       <c r="H151" s="3">
-        <f t="shared" ref="H151" si="149">100*ABS(H150-H146)/H150</f>
+        <f t="shared" ref="H151" si="150">100*ABS(H150-H146)/H150</f>
         <v>24.560132026351415</v>
       </c>
       <c r="I151" s="3">
-        <f t="shared" ref="I151" si="150">100*ABS(I150-I146)/I150</f>
+        <f t="shared" ref="I151" si="151">100*ABS(I150-I146)/I150</f>
         <v>3.1664205479513408</v>
       </c>
       <c r="J151" s="3"/>
       <c r="K151" s="3">
-        <f t="shared" ref="K151" si="151">100*ABS(K150-K146)/K150</f>
+        <f t="shared" ref="K151" si="152">100*ABS(K150-K146)/K150</f>
         <v>10.800908681046586</v>
       </c>
       <c r="L151" s="3">
@@ -18296,48 +18624,48 @@
         <v>1.038399690707694</v>
       </c>
       <c r="C152" s="3">
-        <f t="shared" ref="C152:K152" si="152">100*ABS(C150-C147)/C150</f>
+        <f t="shared" ref="C152:K152" si="153">100*ABS(C150-C147)/C150</f>
         <v>1.3367165870318263</v>
       </c>
       <c r="D152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>5.7084406392648104</v>
       </c>
       <c r="E152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>13.922432441493472</v>
       </c>
       <c r="F152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>14.485325886842576</v>
       </c>
       <c r="G152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>7.2196939678484151</v>
       </c>
       <c r="H152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>9.9117221846807304</v>
       </c>
       <c r="I152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>0.43118057847105945</v>
       </c>
       <c r="J152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>0.54276638721459358</v>
       </c>
       <c r="K152" s="3">
-        <f t="shared" si="152"/>
+        <f t="shared" si="153"/>
         <v>12.217487796787376</v>
       </c>
       <c r="L152" s="3"/>
       <c r="M152" s="3">
-        <f t="shared" ref="M152:M154" si="153">MAX(E152:L152)</f>
+        <f t="shared" ref="M152:M154" si="154">MAX(E152:L152)</f>
         <v>14.485325886842576</v>
       </c>
       <c r="N152" s="3">
-        <f t="shared" ref="N152:N154" si="154">AVERAGE(E152:L152)</f>
+        <f t="shared" ref="N152:N154" si="155">AVERAGE(E152:L152)</f>
         <v>8.3900870347626029</v>
       </c>
     </row>
@@ -18347,39 +18675,39 @@
         <v>1.6770112166657962</v>
       </c>
       <c r="C153" s="3">
-        <f t="shared" ref="C153:K153" si="155">100*ABS(C150-C148)/C150</f>
+        <f t="shared" ref="C153:K153" si="156">100*ABS(C150-C148)/C150</f>
         <v>1.5304751016689389</v>
       </c>
       <c r="D153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>1.4985411762810734</v>
       </c>
       <c r="E153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>1.3557998860122344</v>
       </c>
       <c r="F153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>1.0154499075219015</v>
       </c>
       <c r="G153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>0.48871619686280626</v>
       </c>
       <c r="H153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>6.5552806502243932</v>
       </c>
       <c r="I153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>1.0223507647100176</v>
       </c>
       <c r="J153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>3.1793164227624837</v>
       </c>
       <c r="K153" s="3">
-        <f t="shared" si="155"/>
+        <f t="shared" si="156"/>
         <v>2.3038987634009396</v>
       </c>
       <c r="L153" s="3">
@@ -18387,11 +18715,11 @@
         <v>4.1672599935565788</v>
       </c>
       <c r="M153" s="3">
-        <f t="shared" si="153"/>
+        <f t="shared" si="154"/>
         <v>6.5552806502243932</v>
       </c>
       <c r="N153" s="3">
-        <f t="shared" si="154"/>
+        <f t="shared" si="155"/>
         <v>2.5110090731314192</v>
       </c>
     </row>
@@ -18401,39 +18729,39 @@
         <v>1.3373037270902219</v>
       </c>
       <c r="C154" s="3">
-        <f t="shared" ref="C154:K154" si="156">100*ABS(C150-C149)/C150</f>
+        <f t="shared" ref="C154:K154" si="157">100*ABS(C150-C149)/C150</f>
         <v>1.1570978593906767</v>
       </c>
       <c r="D154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>0.64046287701381521</v>
       </c>
       <c r="E154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>2.5334739288901647</v>
       </c>
       <c r="F154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>2.8993496381399875</v>
       </c>
       <c r="G154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>2.6622472800548325</v>
       </c>
       <c r="H154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>4.9308503907753787</v>
       </c>
       <c r="I154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>3.2616453471617723</v>
       </c>
       <c r="J154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>6.3480984797341335</v>
       </c>
       <c r="K154" s="3">
-        <f t="shared" si="156"/>
+        <f t="shared" si="157"/>
         <v>7.3369729870732803</v>
       </c>
       <c r="L154" s="3">
@@ -18441,11 +18769,11 @@
         <v>14.170633086493584</v>
       </c>
       <c r="M154" s="3">
-        <f t="shared" si="153"/>
+        <f t="shared" si="154"/>
         <v>14.170633086493584</v>
       </c>
       <c r="N154" s="3">
-        <f t="shared" si="154"/>
+        <f t="shared" si="155"/>
         <v>5.5179088922903912</v>
       </c>
     </row>
@@ -18490,42 +18818,42 @@
         <v>0.10145060937534792</v>
       </c>
       <c r="C156" s="2">
-        <f t="shared" ref="C156:L156" si="157">100*ABS(C$155-$E$1 - C146)/C$155</f>
+        <f t="shared" ref="C156:L156" si="158">100*ABS(C$155-$E$1 - C146)/C$155</f>
         <v>1.0966742604318127</v>
       </c>
       <c r="D156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>0.84716178655783902</v>
       </c>
       <c r="E156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>1.8591276834034201</v>
       </c>
       <c r="F156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>3.2864062200276041</v>
       </c>
       <c r="G156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>0.43691215129090988</v>
       </c>
       <c r="H156" s="2"/>
       <c r="I156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>1.0665661956183756</v>
       </c>
       <c r="J156" s="2"/>
       <c r="K156" s="2"/>
       <c r="L156" s="2">
-        <f t="shared" si="157"/>
+        <f t="shared" si="158"/>
         <v>5.3707352764056333</v>
       </c>
       <c r="M156" s="3">
-        <f t="shared" ref="M156" si="158">MAX(E156:L156)</f>
+        <f t="shared" ref="M156" si="159">MAX(E156:L156)</f>
         <v>5.3707352764056333</v>
       </c>
       <c r="N156" s="3">
-        <f t="shared" ref="N156" si="159">AVERAGE(E156:L156)</f>
+        <f t="shared" ref="N156" si="160">AVERAGE(E156:L156)</f>
         <v>2.4039495053491886</v>
       </c>
     </row>
@@ -18534,46 +18862,46 @@
         <v>30</v>
       </c>
       <c r="B157" s="2">
-        <f t="shared" ref="B157:L160" si="160">100*ABS(B$155-$E$1 - B147)/B$155</f>
+        <f t="shared" ref="B157:L160" si="161">100*ABS(B$155-$E$1 - B147)/B$155</f>
         <v>0.14224148296676625</v>
       </c>
       <c r="C157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.8332928240979135</v>
       </c>
       <c r="D157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.2083785321604181</v>
       </c>
       <c r="E157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>2.1920145986544708</v>
       </c>
       <c r="F157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>3.8105867938888869</v>
       </c>
       <c r="G157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.3136618080466593</v>
       </c>
       <c r="H157" s="2"/>
       <c r="I157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.49967584161266032</v>
       </c>
       <c r="J157" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>3.3010003716044434</v>
       </c>
       <c r="K157" s="2"/>
       <c r="L157" s="2"/>
       <c r="M157" s="3">
-        <f t="shared" ref="M157:M160" si="161">MAX(E157:L157)</f>
+        <f t="shared" ref="M157:M160" si="162">MAX(E157:L157)</f>
         <v>3.8105867938888869</v>
       </c>
       <c r="N157" s="3">
-        <f t="shared" ref="N157:N160" si="162">AVERAGE(E157:L157)</f>
+        <f t="shared" ref="N157:N160" si="163">AVERAGE(E157:L157)</f>
         <v>2.2233878827614242</v>
       </c>
     </row>
@@ -18582,49 +18910,49 @@
         <v>40</v>
       </c>
       <c r="B158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.27827187337000037</v>
       </c>
       <c r="C158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.3228064249020559</v>
       </c>
       <c r="D158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>3.6260034139615226E-2</v>
       </c>
       <c r="E158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.2739440645974901</v>
       </c>
       <c r="F158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.87350795448217522</v>
       </c>
       <c r="G158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.12487706643543497</v>
       </c>
       <c r="H158" s="2"/>
       <c r="I158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.19842516273679958</v>
       </c>
       <c r="J158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>2.6541437789756106</v>
       </c>
       <c r="K158" s="2"/>
       <c r="L158" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.11839342175013341</v>
       </c>
       <c r="M158" s="3">
-        <f t="shared" si="161"/>
+        <f t="shared" si="162"/>
         <v>2.6541437789756106</v>
       </c>
       <c r="N158" s="3">
-        <f t="shared" si="162"/>
+        <f t="shared" si="163"/>
         <v>0.70721524149627413</v>
       </c>
     </row>
@@ -18633,49 +18961,49 @@
         <v>50</v>
       </c>
       <c r="B159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.22566416813236601</v>
       </c>
       <c r="C159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.2590599934910558</v>
       </c>
       <c r="D159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.17581490926804688</v>
       </c>
       <c r="E159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>4.2848304002890511E-2</v>
       </c>
       <c r="F159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.2842884281002731</v>
       </c>
       <c r="G159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.50875303141846084</v>
       </c>
       <c r="H159" s="2"/>
       <c r="I159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.26567835751497515</v>
       </c>
       <c r="J159" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>2.1034447030008101</v>
       </c>
       <c r="K159" s="2"/>
       <c r="L159" s="2">
-        <f t="shared" si="160"/>
-        <v>3.2943194918177356</v>
-      </c>
-      <c r="M159" s="3">
         <f t="shared" si="161"/>
         <v>3.2943194918177356</v>
       </c>
+      <c r="M159" s="3">
+        <f t="shared" si="162"/>
+        <v>3.2943194918177356</v>
+      </c>
       <c r="N159" s="3">
-        <f t="shared" si="162"/>
+        <f t="shared" si="163"/>
         <v>1.249888719309191</v>
       </c>
     </row>
@@ -18684,51 +19012,63 @@
         <v>60</v>
       </c>
       <c r="B160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.8566937583078886E-2</v>
       </c>
       <c r="C160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>1.0615094976992103</v>
       </c>
       <c r="D160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.27997756773684096</v>
       </c>
       <c r="E160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.5399935778451429</v>
       </c>
       <c r="F160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.65209118416900913</v>
       </c>
       <c r="G160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>3.8562956126956052E-2</v>
       </c>
       <c r="H160" s="2"/>
       <c r="I160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.41031179549706776</v>
       </c>
       <c r="J160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>3.206673610553886</v>
       </c>
       <c r="K160" s="2"/>
       <c r="L160" s="2">
-        <f t="shared" si="160"/>
+        <f t="shared" si="161"/>
         <v>0.84011808207571781</v>
       </c>
       <c r="M160" s="3">
-        <f t="shared" si="161"/>
+        <f t="shared" si="162"/>
         <v>3.206673610553886</v>
       </c>
       <c r="N160" s="3">
-        <f t="shared" si="162"/>
+        <f t="shared" si="163"/>
         <v>0.9479585343779634</v>
       </c>
+    </row>
+    <row r="161" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B161" s="1"/>
+      <c r="C161" s="1"/>
+      <c r="D161" s="1"/>
+      <c r="E161" s="1"/>
+      <c r="F161" s="1"/>
+      <c r="G161" s="1"/>
+      <c r="H161" s="1"/>
+      <c r="I161" s="1"/>
+      <c r="J161" s="1"/>
+      <c r="K161" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>

</xml_diff>